<commit_message>
abatement a la dream added
</commit_message>
<xml_diff>
--- a/examples/Data/IO/S1.xlsx
+++ b/examples/Data/IO/S1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sxj477\Documents\GitHub\GPM_v4\examples\Data\IO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sxj477\Documents\GitHub\GPM_v05\examples\Data\IO\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="14">
   <si>
     <t>mu/n</t>
   </si>
@@ -54,25 +54,19 @@
     <t>aa_F</t>
   </si>
   <si>
-    <t>b</t>
-  </si>
-  <si>
     <t>bb_F</t>
   </si>
   <si>
     <t>M</t>
   </si>
   <si>
-    <t>a_F</t>
-  </si>
-  <si>
-    <t>b_F</t>
-  </si>
-  <si>
-    <t>iB</t>
-  </si>
-  <si>
-    <t>iM</t>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>X3</t>
   </si>
 </sst>
 </file>
@@ -393,7 +387,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,14 +411,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <f>2/3</f>
-        <v>0.66666666666666663</v>
+        <v>0.25</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -435,17 +428,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3">
-        <f>1-C2</f>
-        <v>0.33333333333333337</v>
+        <v>0.25</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -453,16 +445,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4">
         <v>0.25</v>
@@ -476,8 +468,7 @@
         <v>10</v>
       </c>
       <c r="C5">
-        <f>1-C4</f>
-        <v>0.8</v>
+        <v>0.25</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
@@ -487,45 +478,21 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
       <c r="C6">
         <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
       <c r="C7">
         <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
       <c r="C8">
         <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
       <c r="C9">
         <v>0.5</v>
       </c>
@@ -540,7 +507,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D2" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +531,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>

</xml_diff>